<commit_message>
working rk4 technique with error analysis
</commit_message>
<xml_diff>
--- a/c++/error analysis.xlsx
+++ b/c++/error analysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIP197876\OneDrive - Saipem\Desktop\my-projects\ODE_playground\c++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C258CC91-6606-4D67-991B-D342E75B4CF7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A06E4D9-F299-4B43-B513-B6049AB75E78}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5525F5D3-894A-4421-8A77-FEB4FB74602D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5525F5D3-894A-4421-8A77-FEB4FB74602D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>python</t>
   </si>
@@ -427,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E51A902-C844-4D47-88FC-F58440D41BF0}">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="F103" sqref="F103"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +504,7 @@
         <v>0.19034464388168459</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:F66" si="0">ABS(B3-D3)</f>
+        <f t="shared" ref="E3:E66" si="0">ABS(B3-D3)</f>
         <v>5.8816845838194354E-9</v>
       </c>
       <c r="F3">
@@ -2055,7 +2056,7 @@
         <v>602.98637423593971</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:F101" si="4">ABS(B67-D67)</f>
+        <f t="shared" ref="E67:E101" si="4">ABS(B67-D67)</f>
         <v>6.1764060319546843E-5</v>
       </c>
       <c r="F67">
@@ -2887,6 +2888,2498 @@
       <c r="F102" s="2">
         <f>AVERAGE(F2:F101)</f>
         <v>8.3828434245123145</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:F101">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Trebuchet MS"&amp;8&amp;K22505FSaipem Classification - General Use</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00EB1B13-5764-4C55-8856-8A45CF7E4E59}">
+  <dimension ref="A1:I103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D2" s="1">
+        <f>A2^2 + (1.5*A2) +0.1</f>
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <f>ABS(B2-D2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>ABS(C2-D2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+$I$5</f>
+        <v>5.0505050505050504E-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.17830834000000001</v>
+      </c>
+      <c r="C3">
+        <v>0.17838499999999999</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D66" si="0">A3^2 + (1.5*A3) +0.1</f>
+        <v>0.17830833588409345</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="1">ABS(B3-D3)</f>
+        <v>4.1159065600204769E-9</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="2">ABS(C3-D3)</f>
+        <v>7.6664115906538433E-5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+$I$5</f>
+        <v>0.10101010101010101</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.26171819000000002</v>
+      </c>
+      <c r="C4">
+        <v>0.261965</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26171819202122237</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>2.021222356152208E-9</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>2.4680797877763005E-4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A68" si="3">A4+$I$5</f>
+        <v>0.15151515151515152</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.35022956999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.34987499999999999</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.35022956841138664</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>1.5886133519771306E-9</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>3.5456841138664652E-4</v>
+      </c>
+      <c r="I5">
+        <f>(I3-I2)/(I4-1)</f>
+        <v>5.0505050505050504E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="3"/>
+        <v>0.20202020202020202</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.44384246999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.44231500000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.44384246505458624</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>4.9454137451832025E-9</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>1.5274650545862301E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="3"/>
+        <v>0.25252525252525254</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.54255688000000002</v>
+      </c>
+      <c r="C7">
+        <v>0.53962600000000005</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5425568819508213</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1.9508212822927362E-9</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>2.9308819508212514E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="3"/>
+        <v>0.30303030303030304</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.64637281999999996</v>
+      </c>
+      <c r="C8">
+        <v>0.64209899999999998</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64637281910009181</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>8.9990814799989494E-10</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>4.2738191000918357E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="3"/>
+        <v>0.35353535353535354</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.75529027999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.74968800000000002</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75529027650239766</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>3.4976023188804106E-9</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>5.6022765023976406E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="3"/>
+        <v>0.40404040404040403</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.86930925000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.86214800000000003</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.86930925415773896</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>4.1577389309210844E-9</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>7.1612541577389388E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.98842975</v>
+      </c>
+      <c r="C11">
+        <v>0.97962400000000005</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98842975206611561</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2.066115611931707E-9</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>8.8057520661155575E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>0.50505050505050508</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.11265177</v>
+      </c>
+      <c r="C12">
+        <v>1.1034999999999999</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>1.112651770227528</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>2.2752799644365496E-10</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>9.151770227528111E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.2419753099999999</v>
+      </c>
+      <c r="C13">
+        <v>1.23908</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2419753086419756</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1.3580243596322816E-9</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>2.8953086419756247E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.37640037</v>
+      </c>
+      <c r="C14">
+        <v>1.37984</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3764003673094585</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>2.6905415673184052E-9</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>3.4396326905414831E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="3"/>
+        <v>0.65656565656565657</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.5159269500000001</v>
+      </c>
+      <c r="C15">
+        <v>1.5257799999999999</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5159269462299767</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>3.7700234045701109E-9</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>9.8530537700232124E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="3"/>
+        <v>0.70707070707070707</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.6605550499999999</v>
+      </c>
+      <c r="C16">
+        <v>1.6772899999999999</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6605550454035303</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>4.5964696493427937E-9</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>1.6734954596469676E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="3"/>
+        <v>0.75757575757575757</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1.81028466</v>
+      </c>
+      <c r="C17">
+        <v>1.8347199999999999</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8102846648301192</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>4.8301191934996268E-9</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>2.4435335169880723E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="3"/>
+        <v>0.80808080808080807</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.9651158</v>
+      </c>
+      <c r="C18">
+        <v>1.99732</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9651158045097441</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>4.5097441336849897E-9</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>3.2204195490255882E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="3"/>
+        <v>0.85858585858585856</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.1250484599999999</v>
+      </c>
+      <c r="C19">
+        <v>2.1614599999999999</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1250484644424037</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>4.4424037781709558E-9</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>3.6411535557596242E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="3"/>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.2900826400000001</v>
+      </c>
+      <c r="C20">
+        <v>2.33805</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2900826446280989</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>4.6280987930913398E-9</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>4.796735537190111E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="3"/>
+        <v>0.95959595959595956</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2.4602183499999999</v>
+      </c>
+      <c r="C21">
+        <v>2.5148199999999998</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>2.46021834506683</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>4.9331698726007289E-9</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>5.4601654933169819E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="3"/>
+        <v>1.0101010101010102</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2.63545557</v>
+      </c>
+      <c r="C22">
+        <v>2.6994799999999999</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6354555657585963</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>4.2414036727222992E-9</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>6.4024434241403583E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="3"/>
+        <v>1.0606060606060608</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2.8157943099999998</v>
+      </c>
+      <c r="C23">
+        <v>2.8888699999999998</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8157943067033986</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>3.2966012142310319E-9</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>7.3075693296601241E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="3"/>
+        <v>1.1111111111111114</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3.0012345699999998</v>
+      </c>
+      <c r="C24">
+        <v>3.08161</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0012345679012356</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>2.0987642734837664E-9</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>8.037543209876441E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="3"/>
+        <v>1.161616161616162</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3.19177635</v>
+      </c>
+      <c r="C25">
+        <v>3.2836400000000001</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1917763493521085</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>6.4789151821287305E-10</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>9.1863650647891593E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="3"/>
+        <v>1.2121212121212126</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3.38741965</v>
+      </c>
+      <c r="C26">
+        <v>3.4856600000000002</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3874196510560166</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>1.0560166074924382E-9</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>9.8240348943983591E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="3"/>
+        <v>1.2626262626262632</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3.5881644700000002</v>
+      </c>
+      <c r="C27">
+        <v>3.6991000000000001</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5881644730129607</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>3.0129605477213772E-9</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>0.11093552698703935</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="3"/>
+        <v>1.3131313131313138</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3.79401082</v>
+      </c>
+      <c r="C28">
+        <v>3.9137499999999998</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7940108152229395</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>4.777060524929766E-9</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>0.11973918477706036</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="3"/>
+        <v>1.3636363636363644</v>
+      </c>
+      <c r="B29" s="1">
+        <v>4.0049586799999997</v>
+      </c>
+      <c r="C29">
+        <v>4.1359500000000002</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>4.0049586776859538</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>2.3140458438319911E-9</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>0.13099132231404642</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="3"/>
+        <v>1.414141414141415</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4.22100806</v>
+      </c>
+      <c r="C30">
+        <v>4.3632200000000001</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2210080604020028</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>4.0200287543257218E-10</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>0.14221193959799727</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="3"/>
+        <v>1.4646464646464656</v>
+      </c>
+      <c r="B31" s="1">
+        <v>4.4421589600000004</v>
+      </c>
+      <c r="C31">
+        <v>4.5904999999999996</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4421589633710887</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>3.3710882973991829E-9</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>0.14834103662891085</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="3"/>
+        <v>1.5151515151515162</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4.6684113900000002</v>
+      </c>
+      <c r="C32">
+        <v>4.8178599999999996</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>4.6684113865932098</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>3.4067904053358689E-9</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>0.14944861340678983</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="3"/>
+        <v>1.5656565656565669</v>
+      </c>
+      <c r="B33" s="1">
+        <v>4.8997653300000001</v>
+      </c>
+      <c r="C33">
+        <v>5.0703899999999997</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8997653300683659</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>6.836575749957774E-11</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>0.17062466993163383</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="3"/>
+        <v>1.6161616161616175</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5.1362207900000003</v>
+      </c>
+      <c r="C34">
+        <v>5.3229199999999999</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>5.1362207937965572</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>3.7965568466802324E-9</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>0.18669920620344271</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666681</v>
+      </c>
+      <c r="B35" s="1">
+        <v>5.3777777799999997</v>
+      </c>
+      <c r="C35">
+        <v>5.57545</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>5.3777777777777844</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>2.2222153006623557E-9</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>0.19767222222221559</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="3"/>
+        <v>1.7171717171717187</v>
+      </c>
+      <c r="B36" s="1">
+        <v>5.6244362800000003</v>
+      </c>
+      <c r="C36">
+        <v>5.8279800000000002</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6244362820120468</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>2.0120465293871348E-9</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>0.20354371798795334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="3"/>
+        <v>1.7676767676767693</v>
+      </c>
+      <c r="B37" s="1">
+        <v>5.8761963100000001</v>
+      </c>
+      <c r="C37">
+        <v>6.08765</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8761963064993452</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>3.5006548770866175E-9</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>0.21145369350065479</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="3"/>
+        <v>1.8181818181818199</v>
+      </c>
+      <c r="B38" s="1">
+        <v>6.1330578500000001</v>
+      </c>
+      <c r="C38">
+        <v>6.3654299999999999</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>6.1330578512396778</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>1.2396776938317089E-9</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>0.23237214876032208</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="3"/>
+        <v>1.8686868686868705</v>
+      </c>
+      <c r="B39" s="1">
+        <v>6.3950209200000003</v>
+      </c>
+      <c r="C39">
+        <v>6.6432099999999998</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3950209162330474</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>3.7669529717732075E-9</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>0.24818908376695248</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="3"/>
+        <v>1.9191919191919211</v>
+      </c>
+      <c r="B40" s="1">
+        <v>6.6620854999999999</v>
+      </c>
+      <c r="C40">
+        <v>6.9209899999999998</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6620855014794511</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>1.4794512281923744E-9</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>0.25890449852054864</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="3"/>
+        <v>1.9696969696969717</v>
+      </c>
+      <c r="B41" s="1">
+        <v>6.9342516099999996</v>
+      </c>
+      <c r="C41">
+        <v>7.1987699999999997</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>6.93425160697889</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>3.0211095847221259E-9</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>0.26451839302110969</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="3"/>
+        <v>2.0202020202020221</v>
+      </c>
+      <c r="B42" s="1">
+        <v>7.2115192300000004</v>
+      </c>
+      <c r="C42">
+        <v>7.4907500000000002</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>7.211519232731364</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>2.7313635797554525E-9</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>0.27923076726863627</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="3"/>
+        <v>2.0707070707070727</v>
+      </c>
+      <c r="B43" s="1">
+        <v>7.4938883799999996</v>
+      </c>
+      <c r="C43">
+        <v>7.7937799999999999</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>7.4938883787368749</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>1.2631247159333725E-9</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>0.29989162126312507</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="3"/>
+        <v>2.1212121212121233</v>
+      </c>
+      <c r="B44" s="1">
+        <v>7.7813590499999998</v>
+      </c>
+      <c r="C44">
+        <v>8.0968099999999996</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7813590449954209</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>5.0045789734554091E-9</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>0.31545095500457876</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="3"/>
+        <v>2.1717171717171739</v>
+      </c>
+      <c r="B45" s="1">
+        <v>8.0739312299999995</v>
+      </c>
+      <c r="C45">
+        <v>8.3998500000000007</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="0"/>
+        <v>8.073931231507002</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>1.5070025227714723E-9</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="2"/>
+        <v>0.32591876849299872</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="3"/>
+        <v>2.2222222222222245</v>
+      </c>
+      <c r="B46" s="1">
+        <v>8.3716049399999992</v>
+      </c>
+      <c r="C46">
+        <v>8.7028800000000004</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3716049382716182</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>1.7283809938817285E-9</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="2"/>
+        <v>0.33127506172838217</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="3"/>
+        <v>2.2727272727272751</v>
+      </c>
+      <c r="B47" s="1">
+        <v>8.6743801699999992</v>
+      </c>
+      <c r="C47">
+        <v>9.0059100000000001</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="0"/>
+        <v>8.6743801652892696</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>4.7107295841897212E-9</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
+        <v>0.3315298347107305</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="3"/>
+        <v>2.3232323232323258</v>
+      </c>
+      <c r="B48" s="1">
+        <v>8.9822569100000003</v>
+      </c>
+      <c r="C48">
+        <v>9.3089499999999994</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="0"/>
+        <v>8.9822569125599578</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>2.5599575792512042E-9</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="2"/>
+        <v>0.32669308744004155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="3"/>
+        <v>2.3737373737373764</v>
+      </c>
+      <c r="B49" s="1">
+        <v>9.2952351800000006</v>
+      </c>
+      <c r="C49">
+        <v>9.6362799999999993</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="0"/>
+        <v>9.2952351800836812</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>8.3680617990466999E-11</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="2"/>
+        <v>0.34104481991631808</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="3"/>
+        <v>2.424242424242427</v>
+      </c>
+      <c r="B50" s="1">
+        <v>9.6133149699999993</v>
+      </c>
+      <c r="C50">
+        <v>9.9898199999999999</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="0"/>
+        <v>9.6133149678604379</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>2.1395614169250621E-9</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="2"/>
+        <v>0.37650503213956199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="3"/>
+        <v>2.4747474747474776</v>
+      </c>
+      <c r="B51" s="1">
+        <v>9.9364962800000001</v>
+      </c>
+      <c r="C51">
+        <v>10.343400000000001</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="0"/>
+        <v>9.9364962758902333</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>4.1097667491385437E-9</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="2"/>
+        <v>0.4069037241097675</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="3"/>
+        <v>2.5252525252525282</v>
+      </c>
+      <c r="B52" s="1">
+        <v>10.2647791</v>
+      </c>
+      <c r="C52">
+        <v>10.696899999999999</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="0"/>
+        <v>10.264779104173064</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>4.1730636723968928E-9</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="2"/>
+        <v>0.43212089582693558</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="3"/>
+        <v>2.5757575757575788</v>
+      </c>
+      <c r="B53" s="1">
+        <v>10.598163449999999</v>
+      </c>
+      <c r="C53">
+        <v>11.0504</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="0"/>
+        <v>10.598163452708928</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>2.7089281928738274E-9</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="2"/>
+        <v>0.4522365472910721</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="3"/>
+        <v>2.6262626262626294</v>
+      </c>
+      <c r="B54" s="1">
+        <v>10.936649320000001</v>
+      </c>
+      <c r="C54">
+        <v>11.404</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="0"/>
+        <v>10.936649321497827</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>1.4978258633391306E-9</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="2"/>
+        <v>0.46735067850217327</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="3"/>
+        <v>2.67676767676768</v>
+      </c>
+      <c r="B55" s="1">
+        <v>11.28023671</v>
+      </c>
+      <c r="C55">
+        <v>11.7575</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="0"/>
+        <v>11.280236710539763</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>5.3976201286332071E-10</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="2"/>
+        <v>0.47726328946023777</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="3"/>
+        <v>2.7272727272727306</v>
+      </c>
+      <c r="B56" s="1">
+        <v>11.62892562</v>
+      </c>
+      <c r="C56">
+        <v>12.1111</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="0"/>
+        <v>11.628925619834733</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>1.652669112672811E-10</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="2"/>
+        <v>0.48217438016526692</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="3"/>
+        <v>2.7777777777777812</v>
+      </c>
+      <c r="B57" s="1">
+        <v>11.982716050000001</v>
+      </c>
+      <c r="C57">
+        <v>12.464600000000001</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="0"/>
+        <v>11.98271604938274</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>6.1726090905267483E-10</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="2"/>
+        <v>0.48188395061726119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="3"/>
+        <v>2.8282828282828318</v>
+      </c>
+      <c r="B58" s="1">
+        <v>12.341608000000001</v>
+      </c>
+      <c r="C58">
+        <v>12.8201</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="0"/>
+        <v>12.341607999183781</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="1"/>
+        <v>8.1621998049286049E-10</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="2"/>
+        <v>0.47849200081621923</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="3"/>
+        <v>2.8787878787878824</v>
+      </c>
+      <c r="B59" s="1">
+        <v>12.70560147</v>
+      </c>
+      <c r="C59">
+        <v>13.2242</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="0"/>
+        <v>12.705601469237859</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>7.6214057287415926E-10</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="2"/>
+        <v>0.5185985307621408</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="3"/>
+        <v>2.9292929292929331</v>
+      </c>
+      <c r="B60" s="1">
+        <v>13.07469646</v>
+      </c>
+      <c r="C60">
+        <v>13.6282</v>
+      </c>
+      <c r="D60" s="1">
+        <f t="shared" si="0"/>
+        <v>13.074696459544972</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>4.5502801526708936E-10</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="2"/>
+        <v>0.55350354045502748</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="3"/>
+        <v>2.9797979797979837</v>
+      </c>
+      <c r="B61" s="1">
+        <v>13.448892969999999</v>
+      </c>
+      <c r="C61">
+        <v>14.032299999999999</v>
+      </c>
+      <c r="D61" s="1">
+        <f t="shared" si="0"/>
+        <v>13.448892970105121</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>1.0512124504202802E-10</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="2"/>
+        <v>0.5834070298948788</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="3"/>
+        <v>3.0303030303030343</v>
+      </c>
+      <c r="B62" s="1">
+        <v>13.828191</v>
+      </c>
+      <c r="C62">
+        <v>14.436299999999999</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="0"/>
+        <v>13.828191000918304</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>9.1830365533951408E-10</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="2"/>
+        <v>0.60810899908169525</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="3"/>
+        <v>3.0808080808080849</v>
+      </c>
+      <c r="B63" s="1">
+        <v>14.21259055</v>
+      </c>
+      <c r="C63">
+        <v>14.840400000000001</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="0"/>
+        <v>14.212590551984521</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>1.9845209919822082E-9</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="2"/>
+        <v>0.62780944801547989</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="3"/>
+        <v>3.1313131313131355</v>
+      </c>
+      <c r="B64" s="1">
+        <v>14.602091619999999</v>
+      </c>
+      <c r="C64">
+        <v>15.244400000000001</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="0"/>
+        <v>14.602091623303776</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>3.3037768076837892E-9</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="2"/>
+        <v>0.64230837669622431</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="3"/>
+        <v>3.1818181818181861</v>
+      </c>
+      <c r="B65" s="1">
+        <v>14.996694209999999</v>
+      </c>
+      <c r="C65">
+        <v>15.6485</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="0"/>
+        <v>14.996694214876065</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>4.8760657733737389E-9</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="2"/>
+        <v>0.65180578512393517</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="3"/>
+        <v>3.2323232323232367</v>
+      </c>
+      <c r="B66" s="1">
+        <v>15.39639833</v>
+      </c>
+      <c r="C66">
+        <v>16.052499999999998</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="0"/>
+        <v>15.396398326701391</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>3.2986093856379739E-9</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="2"/>
+        <v>0.65610167329860758</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="3"/>
+        <v>3.2828282828282873</v>
+      </c>
+      <c r="B67" s="1">
+        <v>15.80120396</v>
+      </c>
+      <c r="C67">
+        <v>16.456499999999998</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D101" si="4">A67^2 + (1.5*A67) +0.1</f>
+        <v>15.801203958779752</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E101" si="5">ABS(B67-D67)</f>
+        <v>1.2202487909007687E-9</v>
+      </c>
+      <c r="F67">
+        <f t="shared" ref="F67:F101" si="6">ABS(C67-D67)</f>
+        <v>0.65529604122024665</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333379</v>
+      </c>
+      <c r="B68" s="1">
+        <v>16.211111110000001</v>
+      </c>
+      <c r="C68">
+        <v>16.860600000000002</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="4"/>
+        <v>16.211111111111151</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="5"/>
+        <v>1.1111502828953235E-9</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="6"/>
+        <v>0.64948888888885037</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" ref="A69:A101" si="7">A68+$I$5</f>
+        <v>3.3838383838383885</v>
+      </c>
+      <c r="B69" s="1">
+        <v>16.62611978</v>
+      </c>
+      <c r="C69">
+        <v>17.264600000000002</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="4"/>
+        <v>16.626119783695582</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="5"/>
+        <v>3.6955825066797843E-9</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="6"/>
+        <v>0.6384802163044192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="7"/>
+        <v>3.4343434343434391</v>
+      </c>
+      <c r="B70" s="1">
+        <v>17.04622998</v>
+      </c>
+      <c r="C70">
+        <v>17.668700000000001</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="4"/>
+        <v>17.046229976533049</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="5"/>
+        <v>3.4669511705942568E-9</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="6"/>
+        <v>0.62247002346695268</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="7"/>
+        <v>3.4848484848484897</v>
+      </c>
+      <c r="B71" s="1">
+        <v>17.471441689999999</v>
+      </c>
+      <c r="C71">
+        <v>18.072700000000001</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="4"/>
+        <v>17.47144168962355</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="5"/>
+        <v>3.7644909411937988E-10</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="6"/>
+        <v>0.60125831037645128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="7"/>
+        <v>3.5353535353535404</v>
+      </c>
+      <c r="B72" s="1">
+        <v>17.901754919999998</v>
+      </c>
+      <c r="C72">
+        <v>18.476800000000001</v>
+      </c>
+      <c r="D72" s="1">
+        <f t="shared" si="4"/>
+        <v>17.90175492296709</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="5"/>
+        <v>2.967091461414384E-9</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="6"/>
+        <v>0.57504507703291097</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="7"/>
+        <v>3.585858585858591</v>
+      </c>
+      <c r="B73" s="1">
+        <v>18.337169679999999</v>
+      </c>
+      <c r="C73">
+        <v>18.9695</v>
+      </c>
+      <c r="D73" s="1">
+        <f t="shared" si="4"/>
+        <v>18.337169676563661</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="5"/>
+        <v>3.4363374368240329E-9</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="6"/>
+        <v>0.63233032343633866</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="7"/>
+        <v>3.6363636363636416</v>
+      </c>
+      <c r="B74" s="1">
+        <v>18.777685949999999</v>
+      </c>
+      <c r="C74">
+        <v>19.474499999999999</v>
+      </c>
+      <c r="D74" s="1">
+        <f t="shared" si="4"/>
+        <v>18.777685950413272</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="5"/>
+        <v>4.1327297140014707E-10</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="6"/>
+        <v>0.69681404958672744</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="7"/>
+        <v>3.6868686868686922</v>
+      </c>
+      <c r="B75" s="1">
+        <v>19.223303739999999</v>
+      </c>
+      <c r="C75">
+        <v>19.979600000000001</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="4"/>
+        <v>19.223303744515913</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="5"/>
+        <v>4.5159147532558563E-9</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="6"/>
+        <v>0.75629625548408796</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="7"/>
+        <v>3.7373737373737428</v>
+      </c>
+      <c r="B76" s="1">
+        <v>19.67402306</v>
+      </c>
+      <c r="C76">
+        <v>20.4846</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="4"/>
+        <v>19.674023058871594</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="5"/>
+        <v>1.1284058132332575E-9</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="6"/>
+        <v>0.8105769411284065</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="7"/>
+        <v>3.7878787878787934</v>
+      </c>
+      <c r="B77" s="1">
+        <v>20.12984389</v>
+      </c>
+      <c r="C77">
+        <v>20.989699999999999</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="4"/>
+        <v>20.129843893480309</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="5"/>
+        <v>3.4803093740265467E-9</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="6"/>
+        <v>0.85985610651968969</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="7"/>
+        <v>3.838383838383844</v>
+      </c>
+      <c r="B78" s="1">
+        <v>20.590766250000001</v>
+      </c>
+      <c r="C78">
+        <v>21.494800000000001</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" si="4"/>
+        <v>20.59076624834206</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="5"/>
+        <v>1.657941339772151E-9</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="6"/>
+        <v>0.90403375165794131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="7"/>
+        <v>3.8888888888888946</v>
+      </c>
+      <c r="B79" s="1">
+        <v>21.056790119999999</v>
+      </c>
+      <c r="C79">
+        <v>21.9998</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="4"/>
+        <v>21.056790123456846</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="5"/>
+        <v>3.4568472528917482E-9</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="6"/>
+        <v>0.94300987654315449</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="7"/>
+        <v>3.9393939393939452</v>
+      </c>
+      <c r="B80" s="1">
+        <v>21.527915520000001</v>
+      </c>
+      <c r="C80">
+        <v>22.504899999999999</v>
+      </c>
+      <c r="D80" s="1">
+        <f t="shared" si="4"/>
+        <v>21.527915518824667</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="5"/>
+        <v>1.1753336082165333E-9</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="6"/>
+        <v>0.97698448117533232</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="7"/>
+        <v>3.9898989898989958</v>
+      </c>
+      <c r="B81" s="1">
+        <v>22.004142430000002</v>
+      </c>
+      <c r="C81">
+        <v>23.009899999999998</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="4"/>
+        <v>22.004142434445519</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="5"/>
+        <v>4.4455177317104244E-9</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="6"/>
+        <v>1.0057575655544788</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <f t="shared" si="7"/>
+        <v>4.040404040404046</v>
+      </c>
+      <c r="B82" s="1">
+        <v>22.48547087</v>
+      </c>
+      <c r="C82">
+        <v>23.515000000000001</v>
+      </c>
+      <c r="D82" s="1">
+        <f t="shared" si="4"/>
+        <v>22.485470870319411</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="5"/>
+        <v>3.1941027600623784E-10</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="6"/>
+        <v>1.02952912968059</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <f t="shared" si="7"/>
+        <v>4.0909090909090962</v>
+      </c>
+      <c r="B83" s="1">
+        <v>22.971900829999999</v>
+      </c>
+      <c r="C83">
+        <v>24.02</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" si="4"/>
+        <v>22.971900826446333</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="5"/>
+        <v>3.5536658060664195E-9</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="6"/>
+        <v>1.0480991735536662</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <f t="shared" si="7"/>
+        <v>4.1414141414141463</v>
+      </c>
+      <c r="B84" s="1">
+        <v>23.463432300000001</v>
+      </c>
+      <c r="C84">
+        <v>24.525099999999998</v>
+      </c>
+      <c r="D84" s="1">
+        <f t="shared" si="4"/>
+        <v>23.463432302826291</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="5"/>
+        <v>2.8262903128961625E-9</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="6"/>
+        <v>1.0616676971737071</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" si="7"/>
+        <v>4.1919191919191965</v>
+      </c>
+      <c r="B85" s="1">
+        <v>23.9600653</v>
+      </c>
+      <c r="C85">
+        <v>25.030100000000001</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="4"/>
+        <v>23.960065299459288</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="5"/>
+        <v>5.4071236377239984E-10</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="6"/>
+        <v>1.0700347005407131</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <f t="shared" si="7"/>
+        <v>4.2424242424242466</v>
+      </c>
+      <c r="B86" s="1">
+        <v>24.46179982</v>
+      </c>
+      <c r="C86">
+        <v>25.5352</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="4"/>
+        <v>24.461799816345316</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="5"/>
+        <v>3.6546836668094329E-9</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="6"/>
+        <v>1.0734001836546838</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" si="7"/>
+        <v>4.2929292929292968</v>
+      </c>
+      <c r="B87" s="1">
+        <v>24.968635849999998</v>
+      </c>
+      <c r="C87">
+        <v>26.040299999999998</v>
+      </c>
+      <c r="D87" s="1">
+        <f t="shared" si="4"/>
+        <v>24.968635853484379</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="5"/>
+        <v>3.4843807839024521E-9</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="6"/>
+        <v>1.0716641465156194</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" si="7"/>
+        <v>4.343434343434347</v>
+      </c>
+      <c r="B88" s="1">
+        <v>25.480573410000002</v>
+      </c>
+      <c r="C88">
+        <v>26.545300000000001</v>
+      </c>
+      <c r="D88" s="1">
+        <f t="shared" si="4"/>
+        <v>25.480573410876481</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="5"/>
+        <v>8.7647933355583518E-10</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="6"/>
+        <v>1.06472658912352</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="7"/>
+        <v>4.3939393939393971</v>
+      </c>
+      <c r="B89" s="1">
+        <v>25.997612490000002</v>
+      </c>
+      <c r="C89">
+        <v>27.0504</v>
+      </c>
+      <c r="D89" s="1">
+        <f t="shared" si="4"/>
+        <v>25.997612488521611</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="5"/>
+        <v>1.4783907431592525E-9</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="6"/>
+        <v>1.0527875114783889</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" si="7"/>
+        <v>4.4444444444444473</v>
+      </c>
+      <c r="B90" s="1">
+        <v>26.519753089999998</v>
+      </c>
+      <c r="C90">
+        <v>27.555399999999999</v>
+      </c>
+      <c r="D90" s="1">
+        <f t="shared" si="4"/>
+        <v>26.519753086419783</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="5"/>
+        <v>3.5802152353880956E-9</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="6"/>
+        <v>1.0356469135802158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f t="shared" si="7"/>
+        <v>4.4949494949494975</v>
+      </c>
+      <c r="B91" s="1">
+        <v>27.046995200000001</v>
+      </c>
+      <c r="C91">
+        <v>28.060500000000001</v>
+      </c>
+      <c r="D91" s="1">
+        <f t="shared" si="4"/>
+        <v>27.04699520457099</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="5"/>
+        <v>4.5709889207046217E-9</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="6"/>
+        <v>1.0135047954290108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" si="7"/>
+        <v>4.5454545454545476</v>
+      </c>
+      <c r="B92" s="1">
+        <v>27.579338839999998</v>
+      </c>
+      <c r="C92">
+        <v>28.666</v>
+      </c>
+      <c r="D92" s="1">
+        <f t="shared" si="4"/>
+        <v>27.579338842975233</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="5"/>
+        <v>2.9752342811661947E-9</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="6"/>
+        <v>1.0866611570247677</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <f t="shared" si="7"/>
+        <v>4.5959595959595978</v>
+      </c>
+      <c r="B93" s="1">
+        <v>28.116783999999999</v>
+      </c>
+      <c r="C93">
+        <v>29.272099999999998</v>
+      </c>
+      <c r="D93" s="1">
+        <f t="shared" si="4"/>
+        <v>28.11678400163251</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="5"/>
+        <v>1.632511015259297E-9</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="6"/>
+        <v>1.1553159983674881</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <f t="shared" si="7"/>
+        <v>4.646464646464648</v>
+      </c>
+      <c r="B94" s="1">
+        <v>28.65933068</v>
+      </c>
+      <c r="C94">
+        <v>29.8782</v>
+      </c>
+      <c r="D94" s="1">
+        <f t="shared" si="4"/>
+        <v>28.659330680542819</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="5"/>
+        <v>5.4281912298392854E-10</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="6"/>
+        <v>1.2188693194571805</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <f t="shared" si="7"/>
+        <v>4.6969696969696981</v>
+      </c>
+      <c r="B95" s="1">
+        <v>29.206978880000001</v>
+      </c>
+      <c r="C95">
+        <v>30.484200000000001</v>
+      </c>
+      <c r="D95" s="1">
+        <f t="shared" si="4"/>
+        <v>29.206978879706167</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="5"/>
+        <v>2.9383429023255303E-10</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="6"/>
+        <v>1.2772211202938344</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <f t="shared" si="7"/>
+        <v>4.7474747474747483</v>
+      </c>
+      <c r="B96" s="1">
+        <v>29.759728599999999</v>
+      </c>
+      <c r="C96">
+        <v>31.090299999999999</v>
+      </c>
+      <c r="D96" s="1">
+        <f t="shared" si="4"/>
+        <v>29.759728599122546</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="5"/>
+        <v>8.7745277710382652E-10</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="6"/>
+        <v>1.330571400877453</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <f t="shared" si="7"/>
+        <v>4.7979797979797985</v>
+      </c>
+      <c r="B97" s="1">
+        <v>30.317579840000001</v>
+      </c>
+      <c r="C97">
+        <v>31.696400000000001</v>
+      </c>
+      <c r="D97" s="1">
+        <f t="shared" si="4"/>
+        <v>30.317579838791964</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="5"/>
+        <v>1.2080363376298919E-9</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="6"/>
+        <v>1.3788201612080364</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <f t="shared" si="7"/>
+        <v>4.8484848484848486</v>
+      </c>
+      <c r="B98" s="1">
+        <v>30.880532599999999</v>
+      </c>
+      <c r="C98">
+        <v>32.302399999999999</v>
+      </c>
+      <c r="D98" s="1">
+        <f t="shared" si="4"/>
+        <v>30.880532598714421</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="5"/>
+        <v>1.2855778663833917E-9</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="6"/>
+        <v>1.4218674012855779</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <f t="shared" si="7"/>
+        <v>4.8989898989898988</v>
+      </c>
+      <c r="B99" s="1">
+        <v>31.448586880000001</v>
+      </c>
+      <c r="C99">
+        <v>32.908499999999997</v>
+      </c>
+      <c r="D99" s="1">
+        <f t="shared" si="4"/>
+        <v>31.448586878889909</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="5"/>
+        <v>1.1100915742190409E-9</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="6"/>
+        <v>1.4599131211100875</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <f t="shared" si="7"/>
+        <v>4.9494949494949489</v>
+      </c>
+      <c r="B100" s="1">
+        <v>32.021742680000003</v>
+      </c>
+      <c r="C100">
+        <v>33.514600000000002</v>
+      </c>
+      <c r="D100" s="1">
+        <f t="shared" si="4"/>
+        <v>32.021742679318436</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="5"/>
+        <v>6.815668029958033E-10</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="6"/>
+        <v>1.4928573206815656</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <f t="shared" si="7"/>
+        <v>4.9999999999999991</v>
+      </c>
+      <c r="B101" s="1">
+        <v>32.6</v>
+      </c>
+      <c r="C101">
+        <v>34.120600000000003</v>
+      </c>
+      <c r="D101" s="1">
+        <f t="shared" si="4"/>
+        <v>32.599999999999994</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="5"/>
+        <v>7.1054273576010019E-15</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="6"/>
+        <v>1.5206000000000088</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E102" s="2">
+        <f>AVERAGE(E2:E101)</f>
+        <v>2.3506086455071797E-9</v>
+      </c>
+      <c r="F102" s="2">
+        <f>AVERAGE(F2:F101)</f>
+        <v>0.50090963650135867</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>